<commit_message>
Ajout url extension lieu dit 92edc9862b7f41856ed3270f7b97d411e285a78f
</commit_message>
<xml_diff>
--- a/291-erreur-organization-lieu-dit-precinct/ig/StructureDefinition-as-ext-lieu-dit.xlsx
+++ b/291-erreur-organization-lieu-dit-precinct/ig/StructureDefinition-as-ext-lieu-dit.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://interop.esante.gouv.fr/ig/fhir/ror/StructureDefinition/as-ext-lieu-dit</t>
+    <t>https://interop.esante.gouv.fr/ig/fhir/annuaire/StructureDefinition/as-ext-lieu-dit</t>
   </si>
   <si>
     <t>Version</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-06T13:56:57+00:00</t>
+    <t>2024-02-06T14:47:12+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>